<commit_message>
Web Site - Manual Site without URL - must display name without anchor tag Adding and removing Manual site - New Sites added do not have Enum value - not able to add / remove - solved.
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_2.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="60" yWindow="-45" windowWidth="19470" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Project Number</t>
   </si>
@@ -160,7 +160,10 @@
     <t>0102/0304</t>
   </si>
   <si>
-    <t>0708/0000</t>
+    <t>9002/0000</t>
+  </si>
+  <si>
+    <t>Brazil</t>
   </si>
 </sst>
 </file>
@@ -567,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,6 +682,9 @@
       <c r="I2" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="P2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
added confirm delete modal
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_2.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="-45" windowWidth="19470" windowHeight="7485"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Project Number</t>
   </si>
@@ -85,21 +85,12 @@
     <t>Apollo</t>
   </si>
   <si>
-    <t>some street</t>
-  </si>
-  <si>
-    <t>near to some place</t>
-  </si>
-  <si>
     <t>NY</t>
   </si>
   <si>
     <t>US</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t xml:space="preserve">brown, malcolm d </t>
   </si>
   <si>
@@ -154,16 +145,22 @@
     <t>9002/0000</t>
   </si>
   <si>
+    <t>Robert Jones</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>abc street</t>
+  </si>
+  <si>
     <t>Brazil</t>
   </si>
   <si>
-    <t>Robert Jones</t>
-  </si>
-  <si>
-    <t>Robert</t>
-  </si>
-  <si>
-    <t>Jones</t>
+    <t>Spain</t>
   </si>
 </sst>
 </file>
@@ -570,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,36 +668,36 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="P2" t="s">
         <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -708,7 +705,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
@@ -727,22 +724,20 @@
         <v>22</v>
       </c>
       <c r="K4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="O4" s="2">
         <v>889</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>18</v>
@@ -768,52 +763,52 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="6"/>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" s="6"/>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated UnitOfWork constructor. It now reads two parameters, ConnectionString and DBName Updated the code in required projects when UnitOfWork instance was required
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_2.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_2.xlsx
@@ -22,9 +22,6 @@
     <t>Sponsor Protocol Number</t>
   </si>
   <si>
-    <t>Role (Principal/Sub)</t>
-  </si>
-  <si>
     <t>Member ID</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>Medical License Number</t>
   </si>
   <si>
-    <t>Principal</t>
-  </si>
-  <si>
     <t>#6789</t>
   </si>
   <si>
@@ -100,9 +94,6 @@
     <t>brown</t>
   </si>
   <si>
-    <t>sub</t>
-  </si>
-  <si>
     <t>#11667</t>
   </si>
   <si>
@@ -161,6 +152,15 @@
   </si>
   <si>
     <t>Spain</t>
+  </si>
+  <si>
+    <t>Role (PI/Sub I)</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>sub I</t>
   </si>
 </sst>
 </file>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +612,7 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -621,126 +621,126 @@
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="P2" t="s">
         <v>44</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O4" s="2">
         <v>889</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -763,52 +763,52 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B5" s="6"/>
       <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G5" t="s">
+      <c r="Q5" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B6" s="6"/>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enhacements - QC work flow, two project numbers, admin dashboard, study specific report, findings based report, re-assignment report and time taken to complete a review have been merged and tested
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_2.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Project Number</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>sub I</t>
+  </si>
+  <si>
+    <t>Project Number 2</t>
   </si>
 </sst>
 </file>
@@ -565,52 +568,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI7"/>
+  <dimension ref="A1:AJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5703125" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>46</v>
       </c>
@@ -618,196 +622,209 @@
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>35</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E4" s="2"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="2" t="s">
+      <c r="I5" s="5"/>
+      <c r="J5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3" t="s">
+      <c r="M5" s="2"/>
+      <c r="N5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P5" s="2">
         <v>889</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="Q5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4"/>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>29</v>
+      <c r="C6" s="6"/>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H8" t="s">
         <v>31</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I8" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="J8" s="9" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>